<commit_message>
2021-03-06 debug ProtoGun and Protogen_matrix
</commit_message>
<xml_diff>
--- a/doc/firmware/Remote_CMD.xlsx
+++ b/doc/firmware/Remote_CMD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neil.chuang\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Neil\Protogen\doc\firmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="CMD" sheetId="1" r:id="rId1"/>
     <sheet name="List" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>1X</t>
-  </si>
-  <si>
-    <t>one sound, two sound, random one, random two, random three</t>
   </si>
   <si>
     <t>Pitch up</t>
@@ -189,11 +186,15 @@
   <si>
     <t>Animate</t>
   </si>
+  <si>
+    <t>one sound, two sound, random one, random two, random three, music</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -204,15 +205,18 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -573,7 +577,7 @@
   <dimension ref="A1:AB1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -711,7 +715,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -735,7 +739,7 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>8</v>
@@ -745,7 +749,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="6" t="str">
         <f t="shared" si="0"/>
@@ -784,7 +788,7 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>8</v>
@@ -794,7 +798,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="6" t="str">
         <f t="shared" si="0"/>
@@ -833,7 +837,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
@@ -843,7 +847,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="6" t="str">
         <f t="shared" si="0"/>
@@ -860,7 +864,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -884,7 +888,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>8</v>
@@ -894,7 +898,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="6" t="str">
         <f t="shared" si="0"/>
@@ -911,7 +915,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -965,10 +969,10 @@
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="C9" s="4">
         <f>IF(B9 = List!$A$1, List!$B$1, IF(B9 = List!$A$2, List!$B$2, IF(B9 = List!$A$3, List!$B$3, IF(B9 = List!$A$4, List!$B$4,IF(B9 = List!$A$5, List!$B$5,"")))))</f>
@@ -992,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -1016,17 +1020,17 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="4">
         <f>IF(B10 = List!$A$1, List!$B$1, IF(B10 = List!$A$2, List!$B$2, IF(B10 = List!$A$3, List!$B$3, IF(B10 = List!$A$4, List!$B$4,IF(B10 = List!$A$5, List!$B$5,"")))))</f>
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" s="6" t="str">
         <f t="shared" si="2"/>
@@ -1104,17 +1108,17 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="4">
         <f>IF(B12 = List!$A$1, List!$B$1, IF(B12 = List!$A$2, List!$B$2, IF(B12 = List!$A$3, List!$B$3, IF(B12 = List!$A$4, List!$B$4,IF(B12 = List!$A$5, List!$B$5,"")))))</f>
         <v>1</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="6" t="str">
         <f t="shared" si="2"/>
@@ -1131,7 +1135,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -1194,17 +1198,17 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="4">
         <f>IF(B14 = List!$A$1, List!$B$1, IF(B14 = List!$A$2, List!$B$2, IF(B14 = List!$A$3, List!$B$3, IF(B14 = List!$A$4, List!$B$4,IF(B14 = List!$A$5, List!$B$5,"")))))</f>
         <v>1</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14" s="6" t="str">
         <f t="shared" si="2"/>
@@ -1243,17 +1247,17 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="4">
         <f>IF(B15 = List!$A$1, List!$B$1, IF(B15 = List!$A$2, List!$B$2, IF(B15 = List!$A$3, List!$B$3, IF(B15 = List!$A$4, List!$B$4,IF(B15 = List!$A$5, List!$B$5,"")))))</f>
         <v>1</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" s="6" t="str">
         <f t="shared" si="2"/>
@@ -1331,17 +1335,17 @@
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="4">
         <f>IF(B17 = List!$A$1, List!$B$1, IF(B17 = List!$A$2, List!$B$2, IF(B17 = List!$A$3, List!$B$3, IF(B17 = List!$A$4, List!$B$4,IF(B17 = List!$A$5, List!$B$5,"")))))</f>
         <v>1</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E17" s="6" t="str">
         <f t="shared" si="2"/>
@@ -1358,7 +1362,7 @@
         <v>1</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -1421,17 +1425,17 @@
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="4">
         <f>IF(B19 = List!$A$1, List!$B$1, IF(B19 = List!$A$2, List!$B$2, IF(B19 = List!$A$3, List!$B$3, IF(B19 = List!$A$4, List!$B$4,IF(B19 = List!$A$5, List!$B$5,"")))))</f>
         <v>1</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19" s="6" t="str">
         <f t="shared" si="2"/>
@@ -1448,7 +1452,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -1511,17 +1515,17 @@
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="4">
         <f>IF(B21 = List!$A$1, List!$B$1, IF(B21 = List!$A$2, List!$B$2, IF(B21 = List!$A$3, List!$B$3, IF(B21 = List!$A$4, List!$B$4,IF(B21 = List!$A$5, List!$B$5,"")))))</f>
         <v>1</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" s="6" t="str">
         <f t="shared" si="2"/>
@@ -1538,7 +1542,7 @@
         <v>1</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -1592,10 +1596,10 @@
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="C23" s="4">
         <f>IF(B23 = List!$A$1, List!$B$1, IF(B23 = List!$A$2, List!$B$2, IF(B23 = List!$A$3, List!$B$3, IF(B23 = List!$A$4, List!$B$4,IF(B23 = List!$A$5, List!$B$5,"")))))</f>
@@ -1641,17 +1645,17 @@
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" s="4">
         <f>IF(B24 = List!$A$1, List!$B$1, IF(B24 = List!$A$2, List!$B$2, IF(B24 = List!$A$3, List!$B$3, IF(B24 = List!$A$4, List!$B$4,IF(B24 = List!$A$5, List!$B$5,"")))))</f>
         <v>2</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E24" s="6" t="str">
         <f t="shared" si="4"/>
@@ -1690,17 +1694,17 @@
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" s="4">
         <f>IF(B25 = List!$A$1, List!$B$1, IF(B25 = List!$A$2, List!$B$2, IF(B25 = List!$A$3, List!$B$3, IF(B25 = List!$A$4, List!$B$4,IF(B25 = List!$A$5, List!$B$5,"")))))</f>
         <v>2</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E25" s="6" t="str">
         <f t="shared" si="4"/>
@@ -1739,17 +1743,17 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="4">
         <f>IF(B26 = List!$A$1, List!$B$1, IF(B26 = List!$A$2, List!$B$2, IF(B26 = List!$A$3, List!$B$3, IF(B26 = List!$A$4, List!$B$4,IF(B26 = List!$A$5, List!$B$5,"")))))</f>
         <v>2</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E26" s="6" t="str">
         <f t="shared" si="4"/>
@@ -1827,17 +1831,17 @@
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="C28" s="4">
         <f>IF(B28 = List!$A$1, List!$B$1, IF(B28 = List!$A$2, List!$B$2, IF(B28 = List!$A$3, List!$B$3, IF(B28 = List!$A$4, List!$B$4,IF(B28 = List!$A$5, List!$B$5,"")))))</f>
         <v>3</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E28" s="6" t="str">
         <f t="shared" si="4"/>
@@ -1854,7 +1858,7 @@
         <v>1</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
@@ -39877,7 +39881,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="11">
         <v>1</v>
@@ -39885,7 +39889,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="11">
         <v>2</v>
@@ -39893,7 +39897,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="11">
         <v>3</v>
@@ -39901,7 +39905,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="11">
         <v>4</v>

</xml_diff>